<commit_message>
Update data dictionary and generated synthetic data
</commit_message>
<xml_diff>
--- a/output/input_google_sheets/xlsx/enum_def.xlsx
+++ b/output/input_google_sheets/xlsx/enum_def.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
   <si>
     <t>type_name</t>
   </si>
@@ -109,21 +109,6 @@
     <t>unsure</t>
   </si>
   <si>
-    <t>enum_ms_data_type</t>
-  </si>
-  <si>
-    <t>TIC/XIC</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>MS/MS</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
     <t>enum_table_data_format</t>
   </si>
   <si>
@@ -145,12 +130,15 @@
     <t>mass spec raw</t>
   </si>
   <si>
-    <t>mass spec analysed</t>
+    <t>mass spec processed</t>
   </si>
   <si>
     <t>summarised results</t>
   </si>
   <si>
+    <t>quality control</t>
+  </si>
+  <si>
     <t>enum_instrument_man</t>
   </si>
   <si>
@@ -163,6 +151,9 @@
     <t>Orbitrap Astral</t>
   </si>
   <si>
+    <t>Stellar</t>
+  </si>
+  <si>
     <t>enum_proc_steps</t>
   </si>
   <si>
@@ -182,6 +173,9 @@
   </si>
   <si>
     <t>DIA-NN</t>
+  </si>
+  <si>
+    <t>Skyline</t>
   </si>
 </sst>
 </file>
@@ -230,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -245,6 +239,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -796,6 +793,54 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+      <c r="AG23" s="3"/>
+      <c r="AH23" s="3"/>
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3"/>
+      <c r="AK23" s="3"/>
+      <c r="AL23" s="3"/>
+      <c r="AM23" s="3"/>
+      <c r="AN23" s="3"/>
+      <c r="AO23" s="3"/>
+      <c r="AP23" s="3"/>
+      <c r="AQ23" s="3"/>
+      <c r="AR23" s="3"/>
+      <c r="AS23" s="3"/>
+      <c r="AT23" s="3"/>
+      <c r="AU23" s="3"/>
+      <c r="AV23" s="3"/>
+      <c r="AW23" s="3"/>
+      <c r="AX23" s="3"/>
+      <c r="AY23" s="3"/>
+      <c r="AZ23" s="3"/>
+      <c r="BA23" s="3"/>
+      <c r="BB23" s="3"/>
+      <c r="BC23" s="3"/>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
@@ -809,6 +854,54 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3"/>
+      <c r="AL24" s="3"/>
+      <c r="AM24" s="3"/>
+      <c r="AN24" s="3"/>
+      <c r="AO24" s="3"/>
+      <c r="AP24" s="3"/>
+      <c r="AQ24" s="3"/>
+      <c r="AR24" s="3"/>
+      <c r="AS24" s="3"/>
+      <c r="AT24" s="3"/>
+      <c r="AU24" s="3"/>
+      <c r="AV24" s="3"/>
+      <c r="AW24" s="3"/>
+      <c r="AX24" s="3"/>
+      <c r="AY24" s="3"/>
+      <c r="AZ24" s="3"/>
+      <c r="BA24" s="3"/>
+      <c r="BB24" s="3"/>
+      <c r="BC24" s="3"/>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
@@ -822,6 +915,54 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+      <c r="AG25" s="3"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3"/>
+      <c r="AK25" s="3"/>
+      <c r="AL25" s="3"/>
+      <c r="AM25" s="3"/>
+      <c r="AN25" s="3"/>
+      <c r="AO25" s="3"/>
+      <c r="AP25" s="3"/>
+      <c r="AQ25" s="3"/>
+      <c r="AR25" s="3"/>
+      <c r="AS25" s="3"/>
+      <c r="AT25" s="3"/>
+      <c r="AU25" s="3"/>
+      <c r="AV25" s="3"/>
+      <c r="AW25" s="3"/>
+      <c r="AX25" s="3"/>
+      <c r="AY25" s="3"/>
+      <c r="AZ25" s="3"/>
+      <c r="BA25" s="3"/>
+      <c r="BB25" s="3"/>
+      <c r="BC25" s="3"/>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
@@ -835,12 +976,60 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3"/>
+      <c r="AL26" s="3"/>
+      <c r="AM26" s="3"/>
+      <c r="AN26" s="3"/>
+      <c r="AO26" s="3"/>
+      <c r="AP26" s="3"/>
+      <c r="AQ26" s="3"/>
+      <c r="AR26" s="3"/>
+      <c r="AS26" s="3"/>
+      <c r="AT26" s="3"/>
+      <c r="AU26" s="3"/>
+      <c r="AV26" s="3"/>
+      <c r="AW26" s="3"/>
+      <c r="AX26" s="3"/>
+      <c r="AY26" s="3"/>
+      <c r="AZ26" s="3"/>
+      <c r="BA26" s="3"/>
+      <c r="BB26" s="3"/>
+      <c r="BC26" s="3"/>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C27" s="3"/>
@@ -901,7 +1090,7 @@
       <c r="A28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="3"/>
@@ -1023,300 +1212,80 @@
       <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-      <c r="V30" s="3"/>
-      <c r="W30" s="3"/>
-      <c r="X30" s="3"/>
-      <c r="Y30" s="3"/>
-      <c r="Z30" s="3"/>
-      <c r="AA30" s="3"/>
-      <c r="AB30" s="3"/>
-      <c r="AC30" s="3"/>
-      <c r="AD30" s="3"/>
-      <c r="AE30" s="3"/>
-      <c r="AF30" s="3"/>
-      <c r="AG30" s="3"/>
-      <c r="AH30" s="3"/>
-      <c r="AI30" s="3"/>
-      <c r="AJ30" s="3"/>
-      <c r="AK30" s="3"/>
-      <c r="AL30" s="3"/>
-      <c r="AM30" s="3"/>
-      <c r="AN30" s="3"/>
-      <c r="AO30" s="3"/>
-      <c r="AP30" s="3"/>
-      <c r="AQ30" s="3"/>
-      <c r="AR30" s="3"/>
-      <c r="AS30" s="3"/>
-      <c r="AT30" s="3"/>
-      <c r="AU30" s="3"/>
-      <c r="AV30" s="3"/>
-      <c r="AW30" s="3"/>
-      <c r="AX30" s="3"/>
-      <c r="AY30" s="3"/>
-      <c r="AZ30" s="3"/>
-      <c r="BA30" s="3"/>
-      <c r="BB30" s="3"/>
-      <c r="BC30" s="3"/>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
-      <c r="V31" s="3"/>
-      <c r="W31" s="3"/>
-      <c r="X31" s="3"/>
-      <c r="Y31" s="3"/>
-      <c r="Z31" s="3"/>
-      <c r="AA31" s="3"/>
-      <c r="AB31" s="3"/>
-      <c r="AC31" s="3"/>
-      <c r="AD31" s="3"/>
-      <c r="AE31" s="3"/>
-      <c r="AF31" s="3"/>
-      <c r="AG31" s="3"/>
-      <c r="AH31" s="3"/>
-      <c r="AI31" s="3"/>
-      <c r="AJ31" s="3"/>
-      <c r="AK31" s="3"/>
-      <c r="AL31" s="3"/>
-      <c r="AM31" s="3"/>
-      <c r="AN31" s="3"/>
-      <c r="AO31" s="3"/>
-      <c r="AP31" s="3"/>
-      <c r="AQ31" s="3"/>
-      <c r="AR31" s="3"/>
-      <c r="AS31" s="3"/>
-      <c r="AT31" s="3"/>
-      <c r="AU31" s="3"/>
-      <c r="AV31" s="3"/>
-      <c r="AW31" s="3"/>
-      <c r="AX31" s="3"/>
-      <c r="AY31" s="3"/>
-      <c r="AZ31" s="3"/>
-      <c r="BA31" s="3"/>
-      <c r="BB31" s="3"/>
-      <c r="BC31" s="3"/>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="A32" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
-      <c r="V32" s="3"/>
-      <c r="W32" s="3"/>
-      <c r="X32" s="3"/>
-      <c r="Y32" s="3"/>
-      <c r="Z32" s="3"/>
-      <c r="AA32" s="3"/>
-      <c r="AB32" s="3"/>
-      <c r="AC32" s="3"/>
-      <c r="AD32" s="3"/>
-      <c r="AE32" s="3"/>
-      <c r="AF32" s="3"/>
-      <c r="AG32" s="3"/>
-      <c r="AH32" s="3"/>
-      <c r="AI32" s="3"/>
-      <c r="AJ32" s="3"/>
-      <c r="AK32" s="3"/>
-      <c r="AL32" s="3"/>
-      <c r="AM32" s="3"/>
-      <c r="AN32" s="3"/>
-      <c r="AO32" s="3"/>
-      <c r="AP32" s="3"/>
-      <c r="AQ32" s="3"/>
-      <c r="AR32" s="3"/>
-      <c r="AS32" s="3"/>
-      <c r="AT32" s="3"/>
-      <c r="AU32" s="3"/>
-      <c r="AV32" s="3"/>
-      <c r="AW32" s="3"/>
-      <c r="AX32" s="3"/>
-      <c r="AY32" s="3"/>
-      <c r="AZ32" s="3"/>
-      <c r="BA32" s="3"/>
-      <c r="BB32" s="3"/>
-      <c r="BC32" s="3"/>
+      <c r="B32" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="3"/>
-      <c r="T33" s="3"/>
-      <c r="U33" s="3"/>
-      <c r="V33" s="3"/>
-      <c r="W33" s="3"/>
-      <c r="X33" s="3"/>
-      <c r="Y33" s="3"/>
-      <c r="Z33" s="3"/>
-      <c r="AA33" s="3"/>
-      <c r="AB33" s="3"/>
-      <c r="AC33" s="3"/>
-      <c r="AD33" s="3"/>
-      <c r="AE33" s="3"/>
-      <c r="AF33" s="3"/>
-      <c r="AG33" s="3"/>
-      <c r="AH33" s="3"/>
-      <c r="AI33" s="3"/>
-      <c r="AJ33" s="3"/>
-      <c r="AK33" s="3"/>
-      <c r="AL33" s="3"/>
-      <c r="AM33" s="3"/>
-      <c r="AN33" s="3"/>
-      <c r="AO33" s="3"/>
-      <c r="AP33" s="3"/>
-      <c r="AQ33" s="3"/>
-      <c r="AR33" s="3"/>
-      <c r="AS33" s="3"/>
-      <c r="AT33" s="3"/>
-      <c r="AU33" s="3"/>
-      <c r="AV33" s="3"/>
-      <c r="AW33" s="3"/>
-      <c r="AX33" s="3"/>
-      <c r="AY33" s="3"/>
-      <c r="AZ33" s="3"/>
-      <c r="BA33" s="3"/>
-      <c r="BB33" s="3"/>
-      <c r="BC33" s="3"/>
+      <c r="A33" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="6" t="s">
         <v>47</v>
       </c>
+      <c r="B34" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="5" t="s">
+      <c r="A35" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="5" t="s">
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="5" t="s">
+      <c r="A38" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>